<commit_message>
TSV Y coordinates corrected for origin
</commit_message>
<xml_diff>
--- a/Figure 1/Figure 1(d).xlsx
+++ b/Figure 1/Figure 1(d).xlsx
@@ -36,7 +36,7 @@
     <t>Y-Coordinate_via</t>
   </si>
   <si>
-    <t>Overlap area</t>
+    <t>Designed overlap area</t>
   </si>
 </sst>
 </file>
@@ -420,8 +420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -429,7 +429,7 @@
     <col min="1" max="2" width="8.7265625" style="2"/>
     <col min="3" max="3" width="12.1796875" style="2" customWidth="1"/>
     <col min="4" max="4" width="16.26953125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" style="2"/>
+    <col min="5" max="5" width="18.81640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="18.36328125" style="2" customWidth="1"/>
     <col min="7" max="7" width="15" style="2" customWidth="1"/>
     <col min="8" max="16384" width="8.7265625" style="2"/>

</xml_diff>